<commit_message>
minor update to targets for autoconst
</commit_message>
<xml_diff>
--- a/parameters_targets.xlsx
+++ b/parameters_targets.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="1520" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="33600" windowHeight="19240" tabRatio="500" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="33_targ" sheetId="9" r:id="rId1"/>
     <sheet name="mov_rev_3_targ" sheetId="11" r:id="rId2"/>
-    <sheet name="obs_generator" sheetId="12" r:id="rId3"/>
+    <sheet name="obs_generator_billboard" sheetId="12" r:id="rId3"/>
+    <sheet name="obs_generator_rect_1" sheetId="13" r:id="rId4"/>
+    <sheet name="obs_generator_rect_2" sheetId="14" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="92">
   <si>
     <t>ID</t>
   </si>
@@ -252,6 +254,51 @@
   </si>
   <si>
     <t>cztl.writeObsText(all_fd,'</t>
+  </si>
+  <si>
+    <t>,include_billboard=False)</t>
+  </si>
+  <si>
+    <t>cztl.writeObsTextRect(all_fd,'</t>
+  </si>
+  <si>
+    <t>,upper_lat=</t>
+  </si>
+  <si>
+    <t>,left_long=</t>
+  </si>
+  <si>
+    <t>,right_long=</t>
+  </si>
+  <si>
+    <t>Lower lat</t>
+  </si>
+  <si>
+    <t>Upper lat</t>
+  </si>
+  <si>
+    <t>Left long</t>
+  </si>
+  <si>
+    <t>Right long</t>
+  </si>
+  <si>
+    <t>low lat</t>
+  </si>
+  <si>
+    <t>left long</t>
+  </si>
+  <si>
+    <t>',start_avail,end_avail,color_str='0,255,255,100',lower_lat=</t>
+  </si>
+  <si>
+    <t>HERE</t>
+  </si>
+  <si>
+    <t>Addis Ababa</t>
+  </si>
+  <si>
+    <t>Mount Etna</t>
   </si>
 </sst>
 </file>
@@ -307,7 +354,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -333,12 +380,67 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="79">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -355,6 +457,33 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -363,6 +492,33 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -703,7 +859,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1438,13 +1594,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="C8">
-        <v>46.865918999999998</v>
+        <v>37.749924499999999</v>
       </c>
       <c r="D8">
-        <v>-121.75011000000001</v>
+        <v>14.9894774</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
@@ -1659,13 +1815,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="C21">
-        <v>25.250257000000001</v>
+        <v>8.9631702999999998</v>
       </c>
       <c r="D21">
-        <v>55.339891000000001</v>
+        <v>38.708104499999997</v>
       </c>
       <c r="E21" s="1">
         <v>1</v>
@@ -1795,13 +1951,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>65</v>
+        <v>27</v>
       </c>
       <c r="C29">
-        <v>1.3743399999999999</v>
+        <v>-2.2097019000000002</v>
       </c>
       <c r="D29">
-        <v>103.851294</v>
+        <v>113.8666456</v>
       </c>
       <c r="E29" s="1">
         <v>1</v>
@@ -1941,8 +2097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3258,6 +3414,3388 @@
         <f t="shared" si="1"/>
         <v>cztl.writeObsText(all_fd,'Perth 35',start_avail,end_avail,latitude=-31.91244,longitude=116.738662)</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I50" sqref="I50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>40.705565</v>
+      </c>
+      <c r="C2" s="1">
+        <v>-74.118086599999998</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="1" t="str">
+        <f>CONCATENATE(E2," ",A2)</f>
+        <v>New York 1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2" t="str">
+        <f>CONCATENATE(G2,F2,H2,B2,I2,C2,J2)</f>
+        <v>cztl.writeObsText(all_fd,'New York 1',start_avail,end_avail,latitude=40.705565,longitude=-74.1180866,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>41.833647800000001</v>
+      </c>
+      <c r="C3" s="1">
+        <v>-87.872238400000001</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="1" t="str">
+        <f t="shared" ref="F3:F36" si="0">CONCATENATE(E3," ",A3)</f>
+        <v>Chicago 2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K36" si="1">CONCATENATE(G3,F3,H3,B3,I3,C3,J3)</f>
+        <v>cztl.writeObsText(all_fd,'Chicago 2',start_avail,end_avail,latitude=41.8336478,longitude=-87.8722384,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>33.833765</v>
+      </c>
+      <c r="C4">
+        <v>-117.37276900000001</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>S. California 3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'S. California 3',start_avail,end_avail,latitude=33.833765,longitude=-117.372769,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>36.125230999999999</v>
+      </c>
+      <c r="C5">
+        <v>-119.60391300000001</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Central Valley 4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I5" t="s">
+        <v>74</v>
+      </c>
+      <c r="J5" t="s">
+        <v>77</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'Central Valley 4',start_avail,end_avail,latitude=36.125231,longitude=-119.603913,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>37.783586999999997</v>
+      </c>
+      <c r="C6">
+        <v>-122.420643</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>San Francisco 5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6" t="s">
+        <v>74</v>
+      </c>
+      <c r="J6" t="s">
+        <v>77</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'San Francisco 5',start_avail,end_avail,latitude=37.783587,longitude=-122.420643,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>39.358974000000003</v>
+      </c>
+      <c r="C7">
+        <v>-106.789534</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Colorado 6</v>
+      </c>
+      <c r="G7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" t="s">
+        <v>74</v>
+      </c>
+      <c r="J7" t="s">
+        <v>77</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'Colorado 6',start_avail,end_avail,latitude=39.358974,longitude=-106.789534,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>37.749924499999999</v>
+      </c>
+      <c r="C8">
+        <v>14.9894774</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Mount Etna 7</v>
+      </c>
+      <c r="G8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H8" t="s">
+        <v>73</v>
+      </c>
+      <c r="I8" t="s">
+        <v>74</v>
+      </c>
+      <c r="J8" t="s">
+        <v>77</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'Mount Etna 7',start_avail,end_avail,latitude=37.7499245,longitude=14.9894774,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>23.090699999999998</v>
+      </c>
+      <c r="C9">
+        <v>-82.310919999999996</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Havana 8</v>
+      </c>
+      <c r="G9" t="s">
+        <v>76</v>
+      </c>
+      <c r="H9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I9" t="s">
+        <v>74</v>
+      </c>
+      <c r="J9" t="s">
+        <v>77</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'Havana 8',start_avail,end_avail,latitude=23.0907,longitude=-82.31092,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>-3.1130529999999998</v>
+      </c>
+      <c r="C10">
+        <v>-60.010668000000003</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Amazon 9</v>
+      </c>
+      <c r="G10" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I10" t="s">
+        <v>74</v>
+      </c>
+      <c r="J10" t="s">
+        <v>77</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'Amazon 9',start_avail,end_avail,latitude=-3.113053,longitude=-60.010668,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>-23.404803999999999</v>
+      </c>
+      <c r="C11">
+        <v>-46.858480999999998</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Sao Paulo 10</v>
+      </c>
+      <c r="G11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I11" t="s">
+        <v>74</v>
+      </c>
+      <c r="J11" t="s">
+        <v>77</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'Sao Paulo 10',start_avail,end_avail,latitude=-23.404804,longitude=-46.858481,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>-34.851610000000001</v>
+      </c>
+      <c r="C12">
+        <v>-58.620840999999999</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Buenos Aires 11</v>
+      </c>
+      <c r="G12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H12" t="s">
+        <v>73</v>
+      </c>
+      <c r="I12" t="s">
+        <v>74</v>
+      </c>
+      <c r="J12" t="s">
+        <v>77</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'Buenos Aires 11',start_avail,end_avail,latitude=-34.85161,longitude=-58.620841,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>9.1740239999999993</v>
+      </c>
+      <c r="C13">
+        <v>-79.670525999999995</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Panama Canal 12</v>
+      </c>
+      <c r="G13" t="s">
+        <v>76</v>
+      </c>
+      <c r="H13" t="s">
+        <v>73</v>
+      </c>
+      <c r="I13" t="s">
+        <v>74</v>
+      </c>
+      <c r="J13" t="s">
+        <v>77</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'Panama Canal 12',start_avail,end_avail,latitude=9.174024,longitude=-79.670526,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>48.625622999999997</v>
+      </c>
+      <c r="C14">
+        <v>2.3007219999999999</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Paris 13</v>
+      </c>
+      <c r="G14" t="s">
+        <v>76</v>
+      </c>
+      <c r="H14" t="s">
+        <v>73</v>
+      </c>
+      <c r="I14" t="s">
+        <v>74</v>
+      </c>
+      <c r="J14" t="s">
+        <v>77</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'Paris 13',start_avail,end_avail,latitude=48.625623,longitude=2.300722,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>52.546047000000002</v>
+      </c>
+      <c r="C15">
+        <v>13.321764999999999</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Berlin 14</v>
+      </c>
+      <c r="G15" t="s">
+        <v>76</v>
+      </c>
+      <c r="H15" t="s">
+        <v>73</v>
+      </c>
+      <c r="I15" t="s">
+        <v>74</v>
+      </c>
+      <c r="J15" t="s">
+        <v>77</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'Berlin 14',start_avail,end_avail,latitude=52.546047,longitude=13.321765,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>48.154429999999998</v>
+      </c>
+      <c r="C16">
+        <v>16.375964</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Vienna 15</v>
+      </c>
+      <c r="G16" t="s">
+        <v>76</v>
+      </c>
+      <c r="H16" t="s">
+        <v>73</v>
+      </c>
+      <c r="I16" t="s">
+        <v>74</v>
+      </c>
+      <c r="J16" t="s">
+        <v>77</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'Vienna 15',start_avail,end_avail,latitude=48.15443,longitude=16.375964,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>55.700184</v>
+      </c>
+      <c r="C17">
+        <v>37.686185999999999</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Moscow 16</v>
+      </c>
+      <c r="G17" t="s">
+        <v>76</v>
+      </c>
+      <c r="H17" t="s">
+        <v>73</v>
+      </c>
+      <c r="I17" t="s">
+        <v>74</v>
+      </c>
+      <c r="J17" t="s">
+        <v>77</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'Moscow 16',start_avail,end_avail,latitude=55.700184,longitude=37.686186,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>59.242012000000003</v>
+      </c>
+      <c r="C18">
+        <v>3.505061</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>North Sea 17</v>
+      </c>
+      <c r="G18" t="s">
+        <v>76</v>
+      </c>
+      <c r="H18" t="s">
+        <v>73</v>
+      </c>
+      <c r="I18" t="s">
+        <v>74</v>
+      </c>
+      <c r="J18" t="s">
+        <v>77</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'North Sea 17',start_avail,end_avail,latitude=59.242012,longitude=3.505061,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>30.705666000000001</v>
+      </c>
+      <c r="C19">
+        <v>32.381990999999999</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Suez Canal 18</v>
+      </c>
+      <c r="G19" t="s">
+        <v>76</v>
+      </c>
+      <c r="H19" t="s">
+        <v>73</v>
+      </c>
+      <c r="I19" t="s">
+        <v>74</v>
+      </c>
+      <c r="J19" t="s">
+        <v>77</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'Suez Canal 18',start_avail,end_avail,latitude=30.705666,longitude=32.381991,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>29.588284000000002</v>
+      </c>
+      <c r="C20">
+        <v>49.081795</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Kuwait 19</v>
+      </c>
+      <c r="G20" t="s">
+        <v>76</v>
+      </c>
+      <c r="H20" t="s">
+        <v>73</v>
+      </c>
+      <c r="I20" t="s">
+        <v>74</v>
+      </c>
+      <c r="J20" t="s">
+        <v>77</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'Kuwait 19',start_avail,end_avail,latitude=29.588284,longitude=49.081795,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>8.9631702999999998</v>
+      </c>
+      <c r="C21">
+        <v>38.708104499999997</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>90</v>
+      </c>
+      <c r="F21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Addis Ababa 20</v>
+      </c>
+      <c r="G21" t="s">
+        <v>76</v>
+      </c>
+      <c r="H21" t="s">
+        <v>73</v>
+      </c>
+      <c r="I21" t="s">
+        <v>74</v>
+      </c>
+      <c r="J21" t="s">
+        <v>77</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'Addis Ababa 20',start_avail,end_avail,latitude=8.9631703,longitude=38.7081045,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>6.5204230000000001</v>
+      </c>
+      <c r="C22">
+        <v>3.3797790000000001</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Lagos 21</v>
+      </c>
+      <c r="G22" t="s">
+        <v>76</v>
+      </c>
+      <c r="H22" t="s">
+        <v>73</v>
+      </c>
+      <c r="I22" t="s">
+        <v>74</v>
+      </c>
+      <c r="J22" t="s">
+        <v>77</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'Lagos 21',start_avail,end_avail,latitude=6.520423,longitude=3.379779,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>-2.0240930000000001</v>
+      </c>
+      <c r="C23">
+        <v>22.173711999999998</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>DRC 22</v>
+      </c>
+      <c r="G23" t="s">
+        <v>76</v>
+      </c>
+      <c r="H23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I23" t="s">
+        <v>74</v>
+      </c>
+      <c r="J23" t="s">
+        <v>77</v>
+      </c>
+      <c r="K23" t="str">
+        <f>CONCATENATE(G23,F23,H23,B23,I23,C23,J23)</f>
+        <v>cztl.writeObsText(all_fd,'DRC 22',start_avail,end_avail,latitude=-2.024093,longitude=22.173712,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>-33.872025999999998</v>
+      </c>
+      <c r="C24">
+        <v>18.526935000000002</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>60</v>
+      </c>
+      <c r="F24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Cape Town 23</v>
+      </c>
+      <c r="G24" t="s">
+        <v>76</v>
+      </c>
+      <c r="H24" t="s">
+        <v>73</v>
+      </c>
+      <c r="I24" t="s">
+        <v>74</v>
+      </c>
+      <c r="J24" t="s">
+        <v>77</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'Cape Town 23',start_avail,end_avail,latitude=-33.872026,longitude=18.526935,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>19.004885999999999</v>
+      </c>
+      <c r="C25">
+        <v>72.863435999999993</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Mumbai 24</v>
+      </c>
+      <c r="G25" t="s">
+        <v>76</v>
+      </c>
+      <c r="H25" t="s">
+        <v>73</v>
+      </c>
+      <c r="I25" t="s">
+        <v>74</v>
+      </c>
+      <c r="J25" t="s">
+        <v>77</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'Mumbai 24',start_avail,end_avail,latitude=19.004886,longitude=72.863436,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>28.585252000000001</v>
+      </c>
+      <c r="C26">
+        <v>77.195693000000006</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>New Delhi 25</v>
+      </c>
+      <c r="G26" t="s">
+        <v>76</v>
+      </c>
+      <c r="H26" t="s">
+        <v>73</v>
+      </c>
+      <c r="I26" t="s">
+        <v>74</v>
+      </c>
+      <c r="J26" t="s">
+        <v>77</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'New Delhi 25',start_avail,end_avail,latitude=28.585252,longitude=77.195693,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>23.625858999999998</v>
+      </c>
+      <c r="C27">
+        <v>90.447046999999998</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>63</v>
+      </c>
+      <c r="F27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Dhaka 26</v>
+      </c>
+      <c r="G27" t="s">
+        <v>76</v>
+      </c>
+      <c r="H27" t="s">
+        <v>73</v>
+      </c>
+      <c r="I27" t="s">
+        <v>74</v>
+      </c>
+      <c r="J27" t="s">
+        <v>77</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'Dhaka 26',start_avail,end_avail,latitude=23.625859,longitude=90.447047,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>13.673363999999999</v>
+      </c>
+      <c r="C28">
+        <v>100.95090399999999</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>64</v>
+      </c>
+      <c r="F28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Bangkok 27</v>
+      </c>
+      <c r="G28" t="s">
+        <v>76</v>
+      </c>
+      <c r="H28" t="s">
+        <v>73</v>
+      </c>
+      <c r="I28" t="s">
+        <v>74</v>
+      </c>
+      <c r="J28" t="s">
+        <v>77</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'Bangkok 27',start_avail,end_avail,latitude=13.673364,longitude=100.950904,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>-2.2097019000000002</v>
+      </c>
+      <c r="C29">
+        <v>113.8666456</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Indonesia 28</v>
+      </c>
+      <c r="G29" t="s">
+        <v>76</v>
+      </c>
+      <c r="H29" t="s">
+        <v>73</v>
+      </c>
+      <c r="I29" t="s">
+        <v>74</v>
+      </c>
+      <c r="J29" t="s">
+        <v>77</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'Indonesia 28',start_avail,end_avail,latitude=-2.2097019,longitude=113.8666456,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>22.440325000000001</v>
+      </c>
+      <c r="C30">
+        <v>114.15549799999999</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Hong Kong 29</v>
+      </c>
+      <c r="G30" t="s">
+        <v>76</v>
+      </c>
+      <c r="H30" t="s">
+        <v>73</v>
+      </c>
+      <c r="I30" t="s">
+        <v>74</v>
+      </c>
+      <c r="J30" t="s">
+        <v>77</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'Hong Kong 29',start_avail,end_avail,latitude=22.440325,longitude=114.155498,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>31.240995999999999</v>
+      </c>
+      <c r="C31">
+        <v>121.198994</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31" t="s">
+        <v>66</v>
+      </c>
+      <c r="F31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Shanghai 30</v>
+      </c>
+      <c r="G31" t="s">
+        <v>76</v>
+      </c>
+      <c r="H31" t="s">
+        <v>73</v>
+      </c>
+      <c r="I31" t="s">
+        <v>74</v>
+      </c>
+      <c r="J31" t="s">
+        <v>77</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'Shanghai 30',start_avail,end_avail,latitude=31.240996,longitude=121.198994,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>39.757344000000003</v>
+      </c>
+      <c r="C32">
+        <v>116.36941899999999</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Beijing 31</v>
+      </c>
+      <c r="G32" t="s">
+        <v>76</v>
+      </c>
+      <c r="H32" t="s">
+        <v>73</v>
+      </c>
+      <c r="I32" t="s">
+        <v>74</v>
+      </c>
+      <c r="J32" t="s">
+        <v>77</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'Beijing 31',start_avail,end_avail,latitude=39.757344,longitude=116.369419,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>35.664099</v>
+      </c>
+      <c r="C33">
+        <v>139.50418500000001</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>68</v>
+      </c>
+      <c r="F33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Tokyo 32</v>
+      </c>
+      <c r="G33" t="s">
+        <v>76</v>
+      </c>
+      <c r="H33" t="s">
+        <v>73</v>
+      </c>
+      <c r="I33" t="s">
+        <v>74</v>
+      </c>
+      <c r="J33" t="s">
+        <v>77</v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'Tokyo 32',start_avail,end_avail,latitude=35.664099,longitude=139.504185,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>54.922770999999997</v>
+      </c>
+      <c r="C34">
+        <v>73.898348999999996</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>69</v>
+      </c>
+      <c r="F34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Omsk 33</v>
+      </c>
+      <c r="G34" t="s">
+        <v>76</v>
+      </c>
+      <c r="H34" t="s">
+        <v>73</v>
+      </c>
+      <c r="I34" t="s">
+        <v>74</v>
+      </c>
+      <c r="J34" t="s">
+        <v>77</v>
+      </c>
+      <c r="K34" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'Omsk 33',start_avail,end_avail,latitude=54.922771,longitude=73.898349,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>-33.955050999999997</v>
+      </c>
+      <c r="C35">
+        <v>150.86637200000001</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>70</v>
+      </c>
+      <c r="F35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Sydney 34</v>
+      </c>
+      <c r="G35" t="s">
+        <v>76</v>
+      </c>
+      <c r="H35" t="s">
+        <v>73</v>
+      </c>
+      <c r="I35" t="s">
+        <v>74</v>
+      </c>
+      <c r="J35" t="s">
+        <v>77</v>
+      </c>
+      <c r="K35" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'Sydney 34',start_avail,end_avail,latitude=-33.955051,longitude=150.866372,include_billboard=False)</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>-31.91244</v>
+      </c>
+      <c r="C36">
+        <v>116.73866200000001</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>71</v>
+      </c>
+      <c r="F36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Perth 35</v>
+      </c>
+      <c r="G36" t="s">
+        <v>76</v>
+      </c>
+      <c r="H36" t="s">
+        <v>73</v>
+      </c>
+      <c r="I36" t="s">
+        <v>74</v>
+      </c>
+      <c r="J36" t="s">
+        <v>77</v>
+      </c>
+      <c r="K36" t="str">
+        <f t="shared" si="1"/>
+        <v>cztl.writeObsText(all_fd,'Perth 35',start_avail,end_avail,latitude=-31.91244,longitude=116.738662,include_billboard=False)</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" customWidth="1"/>
+    <col min="12" max="12" width="7.83203125" customWidth="1"/>
+    <col min="15" max="15" width="4.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2">
+        <v>-2</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>-2</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" t="s">
+        <v>85</v>
+      </c>
+      <c r="P4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>40.705565</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-74.118086599999998</v>
+      </c>
+      <c r="D5" s="1">
+        <f>B5+$A$2</f>
+        <v>38.705565</v>
+      </c>
+      <c r="E5" s="1">
+        <f>B5+$B$2</f>
+        <v>42.705565</v>
+      </c>
+      <c r="F5" s="1">
+        <f>C5+$C$2</f>
+        <v>-76.118086599999998</v>
+      </c>
+      <c r="G5" s="1">
+        <f>C5+$D$2</f>
+        <v>-72.118086599999998</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="1" t="str">
+        <f>CONCATENATE(H5," ",A5)</f>
+        <v>New York 1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>78</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L5" t="s">
+        <v>79</v>
+      </c>
+      <c r="M5" t="s">
+        <v>80</v>
+      </c>
+      <c r="N5" t="s">
+        <v>81</v>
+      </c>
+      <c r="O5" t="s">
+        <v>75</v>
+      </c>
+      <c r="P5" t="str">
+        <f>CONCATENATE(J5,I5,K5,D5,L5,E5,M5,F5,N5,G5,O5)</f>
+        <v>cztl.writeObsTextRect(all_fd,'New York 1',start_avail,end_avail,color_str='0,255,255,100',lower_lat=38.705565,upper_lat=42.705565,left_long=-76.1180866,right_long=-72.1180866)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>41.833647800000001</v>
+      </c>
+      <c r="C6" s="1">
+        <v>-87.872238400000001</v>
+      </c>
+      <c r="D6" s="1">
+        <f>B6+$A$2</f>
+        <v>39.833647800000001</v>
+      </c>
+      <c r="E6" s="1">
+        <f>B6+$B$2</f>
+        <v>43.833647800000001</v>
+      </c>
+      <c r="F6" s="1">
+        <f>C6+$C$2</f>
+        <v>-89.872238400000001</v>
+      </c>
+      <c r="G6" s="1">
+        <f>C6+$D$2</f>
+        <v>-85.872238400000001</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="1" t="str">
+        <f>CONCATENATE(H6," ",A6)</f>
+        <v>Chicago 2</v>
+      </c>
+      <c r="J6" t="s">
+        <v>78</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L6" t="s">
+        <v>79</v>
+      </c>
+      <c r="M6" t="s">
+        <v>80</v>
+      </c>
+      <c r="N6" t="s">
+        <v>81</v>
+      </c>
+      <c r="O6" t="s">
+        <v>75</v>
+      </c>
+      <c r="P6" t="str">
+        <f t="shared" ref="P6:P39" si="0">CONCATENATE(J6,I6,K6,D6,L6,E6,M6,F6,N6,G6,O6)</f>
+        <v>cztl.writeObsTextRect(all_fd,'Chicago 2',start_avail,end_avail,color_str='0,255,255,100',lower_lat=39.8336478,upper_lat=43.8336478,left_long=-89.8722384,right_long=-85.8722384)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>33.833765</v>
+      </c>
+      <c r="C7">
+        <v>-117.37276900000001</v>
+      </c>
+      <c r="D7" s="1">
+        <f>B7+$A$2</f>
+        <v>31.833765</v>
+      </c>
+      <c r="E7" s="1">
+        <f>B7+$B$2</f>
+        <v>35.833765</v>
+      </c>
+      <c r="F7" s="1">
+        <f>C7+$C$2</f>
+        <v>-119.37276900000001</v>
+      </c>
+      <c r="G7" s="1">
+        <f>C7+$D$2</f>
+        <v>-115.37276900000001</v>
+      </c>
+      <c r="H7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="1" t="str">
+        <f>CONCATENATE(H7," ",A7)</f>
+        <v>S. California 3</v>
+      </c>
+      <c r="J7" t="s">
+        <v>78</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L7" t="s">
+        <v>79</v>
+      </c>
+      <c r="M7" t="s">
+        <v>80</v>
+      </c>
+      <c r="N7" t="s">
+        <v>81</v>
+      </c>
+      <c r="O7" t="s">
+        <v>75</v>
+      </c>
+      <c r="P7" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'S. California 3',start_avail,end_avail,color_str='0,255,255,100',lower_lat=31.833765,upper_lat=35.833765,left_long=-119.372769,right_long=-115.372769)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="1">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>36.125230999999999</v>
+      </c>
+      <c r="C8">
+        <v>-119.60391300000001</v>
+      </c>
+      <c r="D8" s="1">
+        <f>B8+$A$2</f>
+        <v>34.125230999999999</v>
+      </c>
+      <c r="E8" s="1">
+        <f>B8+$B$2</f>
+        <v>38.125230999999999</v>
+      </c>
+      <c r="F8" s="1">
+        <f>C8+$C$2</f>
+        <v>-121.60391300000001</v>
+      </c>
+      <c r="G8" s="1">
+        <f>C8+$D$2</f>
+        <v>-117.60391300000001</v>
+      </c>
+      <c r="H8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="1" t="str">
+        <f>CONCATENATE(H8," ",A8)</f>
+        <v>Central Valley 4</v>
+      </c>
+      <c r="J8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L8" t="s">
+        <v>79</v>
+      </c>
+      <c r="M8" t="s">
+        <v>80</v>
+      </c>
+      <c r="N8" t="s">
+        <v>81</v>
+      </c>
+      <c r="O8" t="s">
+        <v>75</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'Central Valley 4',start_avail,end_avail,color_str='0,255,255,100',lower_lat=34.125231,upper_lat=38.125231,left_long=-121.603913,right_long=-117.603913)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="1">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>37.783586999999997</v>
+      </c>
+      <c r="C9">
+        <v>-122.420643</v>
+      </c>
+      <c r="D9" s="1">
+        <f>B9+$A$2</f>
+        <v>35.783586999999997</v>
+      </c>
+      <c r="E9" s="1">
+        <f>B9+$B$2</f>
+        <v>39.783586999999997</v>
+      </c>
+      <c r="F9" s="1">
+        <f>C9+$C$2</f>
+        <v>-124.420643</v>
+      </c>
+      <c r="G9" s="1">
+        <f>C9+$D$2</f>
+        <v>-120.420643</v>
+      </c>
+      <c r="H9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="1" t="str">
+        <f>CONCATENATE(H9," ",A9)</f>
+        <v>San Francisco 5</v>
+      </c>
+      <c r="J9" t="s">
+        <v>78</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L9" t="s">
+        <v>79</v>
+      </c>
+      <c r="M9" t="s">
+        <v>80</v>
+      </c>
+      <c r="N9" t="s">
+        <v>81</v>
+      </c>
+      <c r="O9" t="s">
+        <v>75</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'San Francisco 5',start_avail,end_avail,color_str='0,255,255,100',lower_lat=35.783587,upper_lat=39.783587,left_long=-124.420643,right_long=-120.420643)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="1">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>39.358974000000003</v>
+      </c>
+      <c r="C10">
+        <v>-106.789534</v>
+      </c>
+      <c r="D10" s="1">
+        <f>B10+$A$2</f>
+        <v>37.358974000000003</v>
+      </c>
+      <c r="E10" s="1">
+        <f>B10+$B$2</f>
+        <v>41.358974000000003</v>
+      </c>
+      <c r="F10" s="1">
+        <f>C10+$C$2</f>
+        <v>-108.789534</v>
+      </c>
+      <c r="G10" s="1">
+        <f>C10+$D$2</f>
+        <v>-104.789534</v>
+      </c>
+      <c r="H10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="1" t="str">
+        <f>CONCATENATE(H10," ",A10)</f>
+        <v>Colorado 6</v>
+      </c>
+      <c r="J10" t="s">
+        <v>78</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L10" t="s">
+        <v>79</v>
+      </c>
+      <c r="M10" t="s">
+        <v>80</v>
+      </c>
+      <c r="N10" t="s">
+        <v>81</v>
+      </c>
+      <c r="O10" t="s">
+        <v>75</v>
+      </c>
+      <c r="P10" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'Colorado 6',start_avail,end_avail,color_str='0,255,255,100',lower_lat=37.358974,upper_lat=41.358974,left_long=-108.789534,right_long=-104.789534)</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="1">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>37.749924499999999</v>
+      </c>
+      <c r="C11">
+        <v>14.9894774</v>
+      </c>
+      <c r="D11" s="1">
+        <f>B11+$A$2</f>
+        <v>35.749924499999999</v>
+      </c>
+      <c r="E11" s="1">
+        <f>B11+$B$2</f>
+        <v>39.749924499999999</v>
+      </c>
+      <c r="F11" s="1">
+        <f>C11+$C$2</f>
+        <v>12.9894774</v>
+      </c>
+      <c r="G11" s="1">
+        <f>C11+$D$2</f>
+        <v>16.989477399999998</v>
+      </c>
+      <c r="H11" t="s">
+        <v>91</v>
+      </c>
+      <c r="I11" s="1" t="str">
+        <f>CONCATENATE(H11," ",A11)</f>
+        <v>Mount Etna 7</v>
+      </c>
+      <c r="J11" t="s">
+        <v>78</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L11" t="s">
+        <v>79</v>
+      </c>
+      <c r="M11" t="s">
+        <v>80</v>
+      </c>
+      <c r="N11" t="s">
+        <v>81</v>
+      </c>
+      <c r="O11" t="s">
+        <v>75</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'Mount Etna 7',start_avail,end_avail,color_str='0,255,255,100',lower_lat=35.7499245,upper_lat=39.7499245,left_long=12.9894774,right_long=16.9894774)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="1">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>23.090699999999998</v>
+      </c>
+      <c r="C12">
+        <v>-82.310919999999996</v>
+      </c>
+      <c r="D12" s="1">
+        <f>B12+$A$2</f>
+        <v>21.090699999999998</v>
+      </c>
+      <c r="E12" s="1">
+        <f>B12+$B$2</f>
+        <v>25.090699999999998</v>
+      </c>
+      <c r="F12" s="1">
+        <f>C12+$C$2</f>
+        <v>-84.310919999999996</v>
+      </c>
+      <c r="G12" s="1">
+        <f>C12+$D$2</f>
+        <v>-80.310919999999996</v>
+      </c>
+      <c r="H12" t="s">
+        <v>45</v>
+      </c>
+      <c r="I12" s="1" t="str">
+        <f>CONCATENATE(H12," ",A12)</f>
+        <v>Havana 8</v>
+      </c>
+      <c r="J12" t="s">
+        <v>78</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L12" t="s">
+        <v>79</v>
+      </c>
+      <c r="M12" t="s">
+        <v>80</v>
+      </c>
+      <c r="N12" t="s">
+        <v>81</v>
+      </c>
+      <c r="O12" t="s">
+        <v>75</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'Havana 8',start_avail,end_avail,color_str='0,255,255,100',lower_lat=21.0907,upper_lat=25.0907,left_long=-84.31092,right_long=-80.31092)</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="1">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>-3.1130529999999998</v>
+      </c>
+      <c r="C13">
+        <v>-60.010668000000003</v>
+      </c>
+      <c r="D13" s="1">
+        <f>B13+$A$2</f>
+        <v>-5.1130529999999998</v>
+      </c>
+      <c r="E13" s="1">
+        <f>B13+$B$2</f>
+        <v>-1.1130529999999998</v>
+      </c>
+      <c r="F13" s="1">
+        <f>C13+$C$2</f>
+        <v>-62.010668000000003</v>
+      </c>
+      <c r="G13" s="1">
+        <f>C13+$D$2</f>
+        <v>-58.010668000000003</v>
+      </c>
+      <c r="H13" t="s">
+        <v>46</v>
+      </c>
+      <c r="I13" s="1" t="str">
+        <f>CONCATENATE(H13," ",A13)</f>
+        <v>Amazon 9</v>
+      </c>
+      <c r="J13" t="s">
+        <v>78</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L13" t="s">
+        <v>79</v>
+      </c>
+      <c r="M13" t="s">
+        <v>80</v>
+      </c>
+      <c r="N13" t="s">
+        <v>81</v>
+      </c>
+      <c r="O13" t="s">
+        <v>75</v>
+      </c>
+      <c r="P13" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'Amazon 9',start_avail,end_avail,color_str='0,255,255,100',lower_lat=-5.113053,upper_lat=-1.113053,left_long=-62.010668,right_long=-58.010668)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="1">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>-23.404803999999999</v>
+      </c>
+      <c r="C14">
+        <v>-46.858480999999998</v>
+      </c>
+      <c r="D14" s="1">
+        <f>B14+$A$2</f>
+        <v>-25.404803999999999</v>
+      </c>
+      <c r="E14" s="1">
+        <f>B14+$B$2</f>
+        <v>-21.404803999999999</v>
+      </c>
+      <c r="F14" s="1">
+        <f>C14+$C$2</f>
+        <v>-48.858480999999998</v>
+      </c>
+      <c r="G14" s="1">
+        <f>C14+$D$2</f>
+        <v>-44.858480999999998</v>
+      </c>
+      <c r="H14" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" s="1" t="str">
+        <f>CONCATENATE(H14," ",A14)</f>
+        <v>Sao Paulo 10</v>
+      </c>
+      <c r="J14" t="s">
+        <v>78</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L14" t="s">
+        <v>79</v>
+      </c>
+      <c r="M14" t="s">
+        <v>80</v>
+      </c>
+      <c r="N14" t="s">
+        <v>81</v>
+      </c>
+      <c r="O14" t="s">
+        <v>75</v>
+      </c>
+      <c r="P14" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'Sao Paulo 10',start_avail,end_avail,color_str='0,255,255,100',lower_lat=-25.404804,upper_lat=-21.404804,left_long=-48.858481,right_long=-44.858481)</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="1">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>-34.851610000000001</v>
+      </c>
+      <c r="C15">
+        <v>-58.620840999999999</v>
+      </c>
+      <c r="D15" s="1">
+        <f>B15+$A$2</f>
+        <v>-36.851610000000001</v>
+      </c>
+      <c r="E15" s="1">
+        <f>B15+$B$2</f>
+        <v>-32.851610000000001</v>
+      </c>
+      <c r="F15" s="1">
+        <f>C15+$C$2</f>
+        <v>-60.620840999999999</v>
+      </c>
+      <c r="G15" s="1">
+        <f>C15+$D$2</f>
+        <v>-56.620840999999999</v>
+      </c>
+      <c r="H15" t="s">
+        <v>48</v>
+      </c>
+      <c r="I15" s="1" t="str">
+        <f>CONCATENATE(H15," ",A15)</f>
+        <v>Buenos Aires 11</v>
+      </c>
+      <c r="J15" t="s">
+        <v>78</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L15" t="s">
+        <v>79</v>
+      </c>
+      <c r="M15" t="s">
+        <v>80</v>
+      </c>
+      <c r="N15" t="s">
+        <v>81</v>
+      </c>
+      <c r="O15" t="s">
+        <v>75</v>
+      </c>
+      <c r="P15" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'Buenos Aires 11',start_avail,end_avail,color_str='0,255,255,100',lower_lat=-36.85161,upper_lat=-32.85161,left_long=-60.620841,right_long=-56.620841)</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="1">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>9.1740239999999993</v>
+      </c>
+      <c r="C16">
+        <v>-79.670525999999995</v>
+      </c>
+      <c r="D16" s="1">
+        <f>B16+$A$2</f>
+        <v>7.1740239999999993</v>
+      </c>
+      <c r="E16" s="1">
+        <f>B16+$B$2</f>
+        <v>11.174023999999999</v>
+      </c>
+      <c r="F16" s="1">
+        <f>C16+$C$2</f>
+        <v>-81.670525999999995</v>
+      </c>
+      <c r="G16" s="1">
+        <f>C16+$D$2</f>
+        <v>-77.670525999999995</v>
+      </c>
+      <c r="H16" t="s">
+        <v>49</v>
+      </c>
+      <c r="I16" s="1" t="str">
+        <f>CONCATENATE(H16," ",A16)</f>
+        <v>Panama Canal 12</v>
+      </c>
+      <c r="J16" t="s">
+        <v>78</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L16" t="s">
+        <v>79</v>
+      </c>
+      <c r="M16" t="s">
+        <v>80</v>
+      </c>
+      <c r="N16" t="s">
+        <v>81</v>
+      </c>
+      <c r="O16" t="s">
+        <v>75</v>
+      </c>
+      <c r="P16" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'Panama Canal 12',start_avail,end_avail,color_str='0,255,255,100',lower_lat=7.174024,upper_lat=11.174024,left_long=-81.670526,right_long=-77.670526)</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" s="1">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>48.625622999999997</v>
+      </c>
+      <c r="C17">
+        <v>2.3007219999999999</v>
+      </c>
+      <c r="D17" s="1">
+        <f>B17+$A$2</f>
+        <v>46.625622999999997</v>
+      </c>
+      <c r="E17" s="1">
+        <f>B17+$B$2</f>
+        <v>50.625622999999997</v>
+      </c>
+      <c r="F17" s="1">
+        <f>C17+$C$2</f>
+        <v>0.30072199999999993</v>
+      </c>
+      <c r="G17" s="1">
+        <f>C17+$D$2</f>
+        <v>4.3007220000000004</v>
+      </c>
+      <c r="H17" t="s">
+        <v>50</v>
+      </c>
+      <c r="I17" s="1" t="str">
+        <f>CONCATENATE(H17," ",A17)</f>
+        <v>Paris 13</v>
+      </c>
+      <c r="J17" t="s">
+        <v>78</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L17" t="s">
+        <v>79</v>
+      </c>
+      <c r="M17" t="s">
+        <v>80</v>
+      </c>
+      <c r="N17" t="s">
+        <v>81</v>
+      </c>
+      <c r="O17" t="s">
+        <v>75</v>
+      </c>
+      <c r="P17" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'Paris 13',start_avail,end_avail,color_str='0,255,255,100',lower_lat=46.625623,upper_lat=50.625623,left_long=0.300722,right_long=4.300722)</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" s="1">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>52.546047000000002</v>
+      </c>
+      <c r="C18">
+        <v>13.321764999999999</v>
+      </c>
+      <c r="D18" s="1">
+        <f>B18+$A$2</f>
+        <v>50.546047000000002</v>
+      </c>
+      <c r="E18" s="1">
+        <f>B18+$B$2</f>
+        <v>54.546047000000002</v>
+      </c>
+      <c r="F18" s="1">
+        <f>C18+$C$2</f>
+        <v>11.321764999999999</v>
+      </c>
+      <c r="G18" s="1">
+        <f>C18+$D$2</f>
+        <v>15.321764999999999</v>
+      </c>
+      <c r="H18" t="s">
+        <v>51</v>
+      </c>
+      <c r="I18" s="1" t="str">
+        <f>CONCATENATE(H18," ",A18)</f>
+        <v>Berlin 14</v>
+      </c>
+      <c r="J18" t="s">
+        <v>78</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L18" t="s">
+        <v>79</v>
+      </c>
+      <c r="M18" t="s">
+        <v>80</v>
+      </c>
+      <c r="N18" t="s">
+        <v>81</v>
+      </c>
+      <c r="O18" t="s">
+        <v>75</v>
+      </c>
+      <c r="P18" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'Berlin 14',start_avail,end_avail,color_str='0,255,255,100',lower_lat=50.546047,upper_lat=54.546047,left_long=11.321765,right_long=15.321765)</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" s="1">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>48.154429999999998</v>
+      </c>
+      <c r="C19">
+        <v>16.375964</v>
+      </c>
+      <c r="D19" s="1">
+        <f>B19+$A$2</f>
+        <v>46.154429999999998</v>
+      </c>
+      <c r="E19" s="1">
+        <f>B19+$B$2</f>
+        <v>50.154429999999998</v>
+      </c>
+      <c r="F19" s="1">
+        <f>C19+$C$2</f>
+        <v>14.375964</v>
+      </c>
+      <c r="G19" s="1">
+        <f>C19+$D$2</f>
+        <v>18.375964</v>
+      </c>
+      <c r="H19" t="s">
+        <v>52</v>
+      </c>
+      <c r="I19" s="1" t="str">
+        <f>CONCATENATE(H19," ",A19)</f>
+        <v>Vienna 15</v>
+      </c>
+      <c r="J19" t="s">
+        <v>78</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L19" t="s">
+        <v>79</v>
+      </c>
+      <c r="M19" t="s">
+        <v>80</v>
+      </c>
+      <c r="N19" t="s">
+        <v>81</v>
+      </c>
+      <c r="O19" t="s">
+        <v>75</v>
+      </c>
+      <c r="P19" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'Vienna 15',start_avail,end_avail,color_str='0,255,255,100',lower_lat=46.15443,upper_lat=50.15443,left_long=14.375964,right_long=18.375964)</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" s="1">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <v>55.700184</v>
+      </c>
+      <c r="C20">
+        <v>37.686185999999999</v>
+      </c>
+      <c r="D20" s="1">
+        <f>B20+$A$2</f>
+        <v>53.700184</v>
+      </c>
+      <c r="E20" s="1">
+        <f>B20+$B$2</f>
+        <v>57.700184</v>
+      </c>
+      <c r="F20" s="1">
+        <f>C20+$C$2</f>
+        <v>35.686185999999999</v>
+      </c>
+      <c r="G20" s="1">
+        <f>C20+$D$2</f>
+        <v>39.686185999999999</v>
+      </c>
+      <c r="H20" t="s">
+        <v>53</v>
+      </c>
+      <c r="I20" s="1" t="str">
+        <f>CONCATENATE(H20," ",A20)</f>
+        <v>Moscow 16</v>
+      </c>
+      <c r="J20" t="s">
+        <v>78</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L20" t="s">
+        <v>79</v>
+      </c>
+      <c r="M20" t="s">
+        <v>80</v>
+      </c>
+      <c r="N20" t="s">
+        <v>81</v>
+      </c>
+      <c r="O20" t="s">
+        <v>75</v>
+      </c>
+      <c r="P20" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'Moscow 16',start_avail,end_avail,color_str='0,255,255,100',lower_lat=53.700184,upper_lat=57.700184,left_long=35.686186,right_long=39.686186)</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" s="1">
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <v>59.242012000000003</v>
+      </c>
+      <c r="C21">
+        <v>3.505061</v>
+      </c>
+      <c r="D21" s="1">
+        <f>B21+$A$2</f>
+        <v>57.242012000000003</v>
+      </c>
+      <c r="E21" s="1">
+        <f>B21+$B$2</f>
+        <v>61.242012000000003</v>
+      </c>
+      <c r="F21" s="1">
+        <f>C21+$C$2</f>
+        <v>1.505061</v>
+      </c>
+      <c r="G21" s="1">
+        <f>C21+$D$2</f>
+        <v>5.5050609999999995</v>
+      </c>
+      <c r="H21" t="s">
+        <v>54</v>
+      </c>
+      <c r="I21" s="1" t="str">
+        <f>CONCATENATE(H21," ",A21)</f>
+        <v>North Sea 17</v>
+      </c>
+      <c r="J21" t="s">
+        <v>78</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L21" t="s">
+        <v>79</v>
+      </c>
+      <c r="M21" t="s">
+        <v>80</v>
+      </c>
+      <c r="N21" t="s">
+        <v>81</v>
+      </c>
+      <c r="O21" t="s">
+        <v>75</v>
+      </c>
+      <c r="P21" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'North Sea 17',start_avail,end_avail,color_str='0,255,255,100',lower_lat=57.242012,upper_lat=61.242012,left_long=1.505061,right_long=5.505061)</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" s="1">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>30.705666000000001</v>
+      </c>
+      <c r="C22">
+        <v>32.381990999999999</v>
+      </c>
+      <c r="D22" s="1">
+        <f>B22+$A$2</f>
+        <v>28.705666000000001</v>
+      </c>
+      <c r="E22" s="1">
+        <f>B22+$B$2</f>
+        <v>32.705666000000001</v>
+      </c>
+      <c r="F22" s="1">
+        <f>C22+$C$2</f>
+        <v>30.381990999999999</v>
+      </c>
+      <c r="G22" s="1">
+        <f>C22+$D$2</f>
+        <v>34.381990999999999</v>
+      </c>
+      <c r="H22" t="s">
+        <v>55</v>
+      </c>
+      <c r="I22" s="1" t="str">
+        <f>CONCATENATE(H22," ",A22)</f>
+        <v>Suez Canal 18</v>
+      </c>
+      <c r="J22" t="s">
+        <v>78</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L22" t="s">
+        <v>79</v>
+      </c>
+      <c r="M22" t="s">
+        <v>80</v>
+      </c>
+      <c r="N22" t="s">
+        <v>81</v>
+      </c>
+      <c r="O22" t="s">
+        <v>75</v>
+      </c>
+      <c r="P22" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'Suez Canal 18',start_avail,end_avail,color_str='0,255,255,100',lower_lat=28.705666,upper_lat=32.705666,left_long=30.381991,right_long=34.381991)</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" s="1">
+        <v>19</v>
+      </c>
+      <c r="B23">
+        <v>29.588284000000002</v>
+      </c>
+      <c r="C23">
+        <v>49.081795</v>
+      </c>
+      <c r="D23" s="1">
+        <f>B23+$A$2</f>
+        <v>27.588284000000002</v>
+      </c>
+      <c r="E23" s="1">
+        <f>B23+$B$2</f>
+        <v>31.588284000000002</v>
+      </c>
+      <c r="F23" s="1">
+        <f>C23+$C$2</f>
+        <v>47.081795</v>
+      </c>
+      <c r="G23" s="1">
+        <f>C23+$D$2</f>
+        <v>51.081795</v>
+      </c>
+      <c r="H23" t="s">
+        <v>56</v>
+      </c>
+      <c r="I23" s="1" t="str">
+        <f>CONCATENATE(H23," ",A23)</f>
+        <v>Kuwait 19</v>
+      </c>
+      <c r="J23" t="s">
+        <v>78</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L23" t="s">
+        <v>79</v>
+      </c>
+      <c r="M23" t="s">
+        <v>80</v>
+      </c>
+      <c r="N23" t="s">
+        <v>81</v>
+      </c>
+      <c r="O23" t="s">
+        <v>75</v>
+      </c>
+      <c r="P23" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'Kuwait 19',start_avail,end_avail,color_str='0,255,255,100',lower_lat=27.588284,upper_lat=31.588284,left_long=47.081795,right_long=51.081795)</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" s="1">
+        <v>20</v>
+      </c>
+      <c r="B24">
+        <v>8.9631702999999998</v>
+      </c>
+      <c r="C24">
+        <v>38.708104499999997</v>
+      </c>
+      <c r="D24" s="1">
+        <f>B24+$A$2</f>
+        <v>6.9631702999999998</v>
+      </c>
+      <c r="E24" s="1">
+        <f>B24+$B$2</f>
+        <v>10.9631703</v>
+      </c>
+      <c r="F24" s="1">
+        <f>C24+$C$2</f>
+        <v>36.708104499999997</v>
+      </c>
+      <c r="G24" s="1">
+        <f>C24+$D$2</f>
+        <v>40.708104499999997</v>
+      </c>
+      <c r="H24" t="s">
+        <v>90</v>
+      </c>
+      <c r="I24" s="1" t="str">
+        <f>CONCATENATE(H24," ",A24)</f>
+        <v>Addis Ababa 20</v>
+      </c>
+      <c r="J24" t="s">
+        <v>78</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L24" t="s">
+        <v>79</v>
+      </c>
+      <c r="M24" t="s">
+        <v>80</v>
+      </c>
+      <c r="N24" t="s">
+        <v>81</v>
+      </c>
+      <c r="O24" t="s">
+        <v>75</v>
+      </c>
+      <c r="P24" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'Addis Ababa 20',start_avail,end_avail,color_str='0,255,255,100',lower_lat=6.9631703,upper_lat=10.9631703,left_long=36.7081045,right_long=40.7081045)</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" s="1">
+        <v>21</v>
+      </c>
+      <c r="B25">
+        <v>6.5204230000000001</v>
+      </c>
+      <c r="C25">
+        <v>3.3797790000000001</v>
+      </c>
+      <c r="D25" s="1">
+        <f>B25+$A$2</f>
+        <v>4.5204230000000001</v>
+      </c>
+      <c r="E25" s="1">
+        <f>B25+$B$2</f>
+        <v>8.520423000000001</v>
+      </c>
+      <c r="F25" s="1">
+        <f>C25+$C$2</f>
+        <v>1.3797790000000001</v>
+      </c>
+      <c r="G25" s="1">
+        <f>C25+$D$2</f>
+        <v>5.3797790000000001</v>
+      </c>
+      <c r="H25" t="s">
+        <v>58</v>
+      </c>
+      <c r="I25" s="1" t="str">
+        <f>CONCATENATE(H25," ",A25)</f>
+        <v>Lagos 21</v>
+      </c>
+      <c r="J25" t="s">
+        <v>78</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L25" t="s">
+        <v>79</v>
+      </c>
+      <c r="M25" t="s">
+        <v>80</v>
+      </c>
+      <c r="N25" t="s">
+        <v>81</v>
+      </c>
+      <c r="O25" t="s">
+        <v>75</v>
+      </c>
+      <c r="P25" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'Lagos 21',start_avail,end_avail,color_str='0,255,255,100',lower_lat=4.520423,upper_lat=8.520423,left_long=1.379779,right_long=5.379779)</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" s="1">
+        <v>22</v>
+      </c>
+      <c r="B26">
+        <v>-2.0240930000000001</v>
+      </c>
+      <c r="C26">
+        <v>22.173711999999998</v>
+      </c>
+      <c r="D26" s="1">
+        <f>B26+$A$2</f>
+        <v>-4.0240930000000006</v>
+      </c>
+      <c r="E26" s="1">
+        <f>B26+$B$2</f>
+        <v>-2.4093000000000142E-2</v>
+      </c>
+      <c r="F26" s="1">
+        <f>C26+$C$2</f>
+        <v>20.173711999999998</v>
+      </c>
+      <c r="G26" s="1">
+        <f>C26+$D$2</f>
+        <v>24.173711999999998</v>
+      </c>
+      <c r="H26" t="s">
+        <v>59</v>
+      </c>
+      <c r="I26" s="1" t="str">
+        <f>CONCATENATE(H26," ",A26)</f>
+        <v>DRC 22</v>
+      </c>
+      <c r="J26" t="s">
+        <v>78</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L26" t="s">
+        <v>79</v>
+      </c>
+      <c r="M26" t="s">
+        <v>80</v>
+      </c>
+      <c r="N26" t="s">
+        <v>81</v>
+      </c>
+      <c r="O26" t="s">
+        <v>75</v>
+      </c>
+      <c r="P26" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'DRC 22',start_avail,end_avail,color_str='0,255,255,100',lower_lat=-4.024093,upper_lat=-0.0240930000000001,left_long=20.173712,right_long=24.173712)</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" s="1">
+        <v>23</v>
+      </c>
+      <c r="B27">
+        <v>-33.872025999999998</v>
+      </c>
+      <c r="C27">
+        <v>18.526935000000002</v>
+      </c>
+      <c r="D27" s="1">
+        <f>B27+$A$2</f>
+        <v>-35.872025999999998</v>
+      </c>
+      <c r="E27" s="1">
+        <f>B27+$B$2</f>
+        <v>-31.872025999999998</v>
+      </c>
+      <c r="F27" s="1">
+        <f>C27+$C$2</f>
+        <v>16.526935000000002</v>
+      </c>
+      <c r="G27" s="1">
+        <f>C27+$D$2</f>
+        <v>20.526935000000002</v>
+      </c>
+      <c r="H27" t="s">
+        <v>60</v>
+      </c>
+      <c r="I27" s="1" t="str">
+        <f>CONCATENATE(H27," ",A27)</f>
+        <v>Cape Town 23</v>
+      </c>
+      <c r="J27" t="s">
+        <v>78</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L27" t="s">
+        <v>79</v>
+      </c>
+      <c r="M27" t="s">
+        <v>80</v>
+      </c>
+      <c r="N27" t="s">
+        <v>81</v>
+      </c>
+      <c r="O27" t="s">
+        <v>75</v>
+      </c>
+      <c r="P27" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'Cape Town 23',start_avail,end_avail,color_str='0,255,255,100',lower_lat=-35.872026,upper_lat=-31.872026,left_long=16.526935,right_long=20.526935)</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" s="1">
+        <v>24</v>
+      </c>
+      <c r="B28">
+        <v>19.004885999999999</v>
+      </c>
+      <c r="C28">
+        <v>72.863435999999993</v>
+      </c>
+      <c r="D28" s="1">
+        <f>B28+$A$2</f>
+        <v>17.004885999999999</v>
+      </c>
+      <c r="E28" s="1">
+        <f>B28+$B$2</f>
+        <v>21.004885999999999</v>
+      </c>
+      <c r="F28" s="1">
+        <f>C28+$C$2</f>
+        <v>70.863435999999993</v>
+      </c>
+      <c r="G28" s="1">
+        <f>C28+$D$2</f>
+        <v>74.863435999999993</v>
+      </c>
+      <c r="H28" t="s">
+        <v>61</v>
+      </c>
+      <c r="I28" s="1" t="str">
+        <f>CONCATENATE(H28," ",A28)</f>
+        <v>Mumbai 24</v>
+      </c>
+      <c r="J28" t="s">
+        <v>78</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L28" t="s">
+        <v>79</v>
+      </c>
+      <c r="M28" t="s">
+        <v>80</v>
+      </c>
+      <c r="N28" t="s">
+        <v>81</v>
+      </c>
+      <c r="O28" t="s">
+        <v>75</v>
+      </c>
+      <c r="P28" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'Mumbai 24',start_avail,end_avail,color_str='0,255,255,100',lower_lat=17.004886,upper_lat=21.004886,left_long=70.863436,right_long=74.863436)</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" s="1">
+        <v>25</v>
+      </c>
+      <c r="B29">
+        <v>28.585252000000001</v>
+      </c>
+      <c r="C29">
+        <v>77.195693000000006</v>
+      </c>
+      <c r="D29" s="1">
+        <f>B29+$A$2</f>
+        <v>26.585252000000001</v>
+      </c>
+      <c r="E29" s="1">
+        <f>B29+$B$2</f>
+        <v>30.585252000000001</v>
+      </c>
+      <c r="F29" s="1">
+        <f>C29+$C$2</f>
+        <v>75.195693000000006</v>
+      </c>
+      <c r="G29" s="1">
+        <f>C29+$D$2</f>
+        <v>79.195693000000006</v>
+      </c>
+      <c r="H29" t="s">
+        <v>62</v>
+      </c>
+      <c r="I29" s="1" t="str">
+        <f>CONCATENATE(H29," ",A29)</f>
+        <v>New Delhi 25</v>
+      </c>
+      <c r="J29" t="s">
+        <v>78</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L29" t="s">
+        <v>79</v>
+      </c>
+      <c r="M29" t="s">
+        <v>80</v>
+      </c>
+      <c r="N29" t="s">
+        <v>81</v>
+      </c>
+      <c r="O29" t="s">
+        <v>75</v>
+      </c>
+      <c r="P29" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'New Delhi 25',start_avail,end_avail,color_str='0,255,255,100',lower_lat=26.585252,upper_lat=30.585252,left_long=75.195693,right_long=79.195693)</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" s="1">
+        <v>26</v>
+      </c>
+      <c r="B30">
+        <v>23.625858999999998</v>
+      </c>
+      <c r="C30">
+        <v>90.447046999999998</v>
+      </c>
+      <c r="D30" s="1">
+        <f>B30+$A$2</f>
+        <v>21.625858999999998</v>
+      </c>
+      <c r="E30" s="1">
+        <f>B30+$B$2</f>
+        <v>25.625858999999998</v>
+      </c>
+      <c r="F30" s="1">
+        <f>C30+$C$2</f>
+        <v>88.447046999999998</v>
+      </c>
+      <c r="G30" s="1">
+        <f>C30+$D$2</f>
+        <v>92.447046999999998</v>
+      </c>
+      <c r="H30" t="s">
+        <v>63</v>
+      </c>
+      <c r="I30" s="1" t="str">
+        <f>CONCATENATE(H30," ",A30)</f>
+        <v>Dhaka 26</v>
+      </c>
+      <c r="J30" t="s">
+        <v>78</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L30" t="s">
+        <v>79</v>
+      </c>
+      <c r="M30" t="s">
+        <v>80</v>
+      </c>
+      <c r="N30" t="s">
+        <v>81</v>
+      </c>
+      <c r="O30" t="s">
+        <v>75</v>
+      </c>
+      <c r="P30" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'Dhaka 26',start_avail,end_avail,color_str='0,255,255,100',lower_lat=21.625859,upper_lat=25.625859,left_long=88.447047,right_long=92.447047)</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" s="1">
+        <v>27</v>
+      </c>
+      <c r="B31">
+        <v>13.673363999999999</v>
+      </c>
+      <c r="C31">
+        <v>100.95090399999999</v>
+      </c>
+      <c r="D31" s="1">
+        <f>B31+$A$2</f>
+        <v>11.673363999999999</v>
+      </c>
+      <c r="E31" s="1">
+        <f>B31+$B$2</f>
+        <v>15.673363999999999</v>
+      </c>
+      <c r="F31" s="1">
+        <f>C31+$C$2</f>
+        <v>98.950903999999994</v>
+      </c>
+      <c r="G31" s="1">
+        <f>C31+$D$2</f>
+        <v>102.95090399999999</v>
+      </c>
+      <c r="H31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I31" s="1" t="str">
+        <f>CONCATENATE(H31," ",A31)</f>
+        <v>Bangkok 27</v>
+      </c>
+      <c r="J31" t="s">
+        <v>78</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L31" t="s">
+        <v>79</v>
+      </c>
+      <c r="M31" t="s">
+        <v>80</v>
+      </c>
+      <c r="N31" t="s">
+        <v>81</v>
+      </c>
+      <c r="O31" t="s">
+        <v>75</v>
+      </c>
+      <c r="P31" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'Bangkok 27',start_avail,end_avail,color_str='0,255,255,100',lower_lat=11.673364,upper_lat=15.673364,left_long=98.950904,right_long=102.950904)</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32" s="1">
+        <v>28</v>
+      </c>
+      <c r="B32">
+        <v>-2.2097019000000002</v>
+      </c>
+      <c r="C32">
+        <v>113.8666456</v>
+      </c>
+      <c r="D32" s="1">
+        <f>B32+$A$2</f>
+        <v>-4.2097019000000007</v>
+      </c>
+      <c r="E32" s="1">
+        <f>B32+$B$2</f>
+        <v>-0.20970190000000022</v>
+      </c>
+      <c r="F32" s="1">
+        <f>C32+$C$2</f>
+        <v>111.8666456</v>
+      </c>
+      <c r="G32" s="1">
+        <f>C32+$D$2</f>
+        <v>115.8666456</v>
+      </c>
+      <c r="H32" t="s">
+        <v>27</v>
+      </c>
+      <c r="I32" s="1" t="str">
+        <f>CONCATENATE(H32," ",A32)</f>
+        <v>Indonesia 28</v>
+      </c>
+      <c r="J32" t="s">
+        <v>78</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L32" t="s">
+        <v>79</v>
+      </c>
+      <c r="M32" t="s">
+        <v>80</v>
+      </c>
+      <c r="N32" t="s">
+        <v>81</v>
+      </c>
+      <c r="O32" t="s">
+        <v>75</v>
+      </c>
+      <c r="P32" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'Indonesia 28',start_avail,end_avail,color_str='0,255,255,100',lower_lat=-4.2097019,upper_lat=-0.2097019,left_long=111.8666456,right_long=115.8666456)</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" s="1">
+        <v>29</v>
+      </c>
+      <c r="B33">
+        <v>22.440325000000001</v>
+      </c>
+      <c r="C33">
+        <v>114.15549799999999</v>
+      </c>
+      <c r="D33" s="1">
+        <f>B33+$A$2</f>
+        <v>20.440325000000001</v>
+      </c>
+      <c r="E33" s="1">
+        <f>B33+$B$2</f>
+        <v>24.440325000000001</v>
+      </c>
+      <c r="F33" s="1">
+        <f>C33+$C$2</f>
+        <v>112.15549799999999</v>
+      </c>
+      <c r="G33" s="1">
+        <f>C33+$D$2</f>
+        <v>116.15549799999999</v>
+      </c>
+      <c r="H33" t="s">
+        <v>32</v>
+      </c>
+      <c r="I33" s="1" t="str">
+        <f>CONCATENATE(H33," ",A33)</f>
+        <v>Hong Kong 29</v>
+      </c>
+      <c r="J33" t="s">
+        <v>78</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L33" t="s">
+        <v>79</v>
+      </c>
+      <c r="M33" t="s">
+        <v>80</v>
+      </c>
+      <c r="N33" t="s">
+        <v>81</v>
+      </c>
+      <c r="O33" t="s">
+        <v>75</v>
+      </c>
+      <c r="P33" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'Hong Kong 29',start_avail,end_avail,color_str='0,255,255,100',lower_lat=20.440325,upper_lat=24.440325,left_long=112.155498,right_long=116.155498)</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34" s="1">
+        <v>30</v>
+      </c>
+      <c r="B34">
+        <v>31.240995999999999</v>
+      </c>
+      <c r="C34">
+        <v>121.198994</v>
+      </c>
+      <c r="D34" s="1">
+        <f>B34+$A$2</f>
+        <v>29.240995999999999</v>
+      </c>
+      <c r="E34" s="1">
+        <f>B34+$B$2</f>
+        <v>33.240995999999996</v>
+      </c>
+      <c r="F34" s="1">
+        <f>C34+$C$2</f>
+        <v>119.198994</v>
+      </c>
+      <c r="G34" s="1">
+        <f>C34+$D$2</f>
+        <v>123.198994</v>
+      </c>
+      <c r="H34" t="s">
+        <v>66</v>
+      </c>
+      <c r="I34" s="1" t="str">
+        <f>CONCATENATE(H34," ",A34)</f>
+        <v>Shanghai 30</v>
+      </c>
+      <c r="J34" t="s">
+        <v>78</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L34" t="s">
+        <v>79</v>
+      </c>
+      <c r="M34" t="s">
+        <v>80</v>
+      </c>
+      <c r="N34" t="s">
+        <v>81</v>
+      </c>
+      <c r="O34" t="s">
+        <v>75</v>
+      </c>
+      <c r="P34" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'Shanghai 30',start_avail,end_avail,color_str='0,255,255,100',lower_lat=29.240996,upper_lat=33.240996,left_long=119.198994,right_long=123.198994)</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="A35" s="1">
+        <v>31</v>
+      </c>
+      <c r="B35">
+        <v>39.757344000000003</v>
+      </c>
+      <c r="C35">
+        <v>116.36941899999999</v>
+      </c>
+      <c r="D35" s="1">
+        <f>B35+$A$2</f>
+        <v>37.757344000000003</v>
+      </c>
+      <c r="E35" s="1">
+        <f>B35+$B$2</f>
+        <v>41.757344000000003</v>
+      </c>
+      <c r="F35" s="1">
+        <f>C35+$C$2</f>
+        <v>114.36941899999999</v>
+      </c>
+      <c r="G35" s="1">
+        <f>C35+$D$2</f>
+        <v>118.36941899999999</v>
+      </c>
+      <c r="H35" t="s">
+        <v>67</v>
+      </c>
+      <c r="I35" s="1" t="str">
+        <f>CONCATENATE(H35," ",A35)</f>
+        <v>Beijing 31</v>
+      </c>
+      <c r="J35" t="s">
+        <v>78</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L35" t="s">
+        <v>79</v>
+      </c>
+      <c r="M35" t="s">
+        <v>80</v>
+      </c>
+      <c r="N35" t="s">
+        <v>81</v>
+      </c>
+      <c r="O35" t="s">
+        <v>75</v>
+      </c>
+      <c r="P35" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'Beijing 31',start_avail,end_avail,color_str='0,255,255,100',lower_lat=37.757344,upper_lat=41.757344,left_long=114.369419,right_long=118.369419)</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
+      <c r="A36" s="1">
+        <v>32</v>
+      </c>
+      <c r="B36">
+        <v>35.664099</v>
+      </c>
+      <c r="C36">
+        <v>139.50418500000001</v>
+      </c>
+      <c r="D36" s="1">
+        <f>B36+$A$2</f>
+        <v>33.664099</v>
+      </c>
+      <c r="E36" s="1">
+        <f>B36+$B$2</f>
+        <v>37.664099</v>
+      </c>
+      <c r="F36" s="1">
+        <f>C36+$C$2</f>
+        <v>137.50418500000001</v>
+      </c>
+      <c r="G36" s="1">
+        <f>C36+$D$2</f>
+        <v>141.50418500000001</v>
+      </c>
+      <c r="H36" t="s">
+        <v>68</v>
+      </c>
+      <c r="I36" s="1" t="str">
+        <f>CONCATENATE(H36," ",A36)</f>
+        <v>Tokyo 32</v>
+      </c>
+      <c r="J36" t="s">
+        <v>78</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L36" t="s">
+        <v>79</v>
+      </c>
+      <c r="M36" t="s">
+        <v>80</v>
+      </c>
+      <c r="N36" t="s">
+        <v>81</v>
+      </c>
+      <c r="O36" t="s">
+        <v>75</v>
+      </c>
+      <c r="P36" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'Tokyo 32',start_avail,end_avail,color_str='0,255,255,100',lower_lat=33.664099,upper_lat=37.664099,left_long=137.504185,right_long=141.504185)</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
+      <c r="A37" s="1">
+        <v>33</v>
+      </c>
+      <c r="B37">
+        <v>54.922770999999997</v>
+      </c>
+      <c r="C37">
+        <v>73.898348999999996</v>
+      </c>
+      <c r="D37" s="1">
+        <f>B37+$A$2</f>
+        <v>52.922770999999997</v>
+      </c>
+      <c r="E37" s="1">
+        <f>B37+$B$2</f>
+        <v>56.922770999999997</v>
+      </c>
+      <c r="F37" s="1">
+        <f>C37+$C$2</f>
+        <v>71.898348999999996</v>
+      </c>
+      <c r="G37" s="1">
+        <f>C37+$D$2</f>
+        <v>75.898348999999996</v>
+      </c>
+      <c r="H37" t="s">
+        <v>69</v>
+      </c>
+      <c r="I37" s="1" t="str">
+        <f>CONCATENATE(H37," ",A37)</f>
+        <v>Omsk 33</v>
+      </c>
+      <c r="J37" t="s">
+        <v>78</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L37" t="s">
+        <v>79</v>
+      </c>
+      <c r="M37" t="s">
+        <v>80</v>
+      </c>
+      <c r="N37" t="s">
+        <v>81</v>
+      </c>
+      <c r="O37" t="s">
+        <v>75</v>
+      </c>
+      <c r="P37" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'Omsk 33',start_avail,end_avail,color_str='0,255,255,100',lower_lat=52.922771,upper_lat=56.922771,left_long=71.898349,right_long=75.898349)</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
+      <c r="A38" s="1">
+        <v>34</v>
+      </c>
+      <c r="B38">
+        <v>-33.955050999999997</v>
+      </c>
+      <c r="C38">
+        <v>150.86637200000001</v>
+      </c>
+      <c r="D38" s="1">
+        <f>B38+$A$2</f>
+        <v>-35.955050999999997</v>
+      </c>
+      <c r="E38" s="1">
+        <f>B38+$B$2</f>
+        <v>-31.955050999999997</v>
+      </c>
+      <c r="F38" s="1">
+        <f>C38+$C$2</f>
+        <v>148.86637200000001</v>
+      </c>
+      <c r="G38" s="1">
+        <f>C38+$D$2</f>
+        <v>152.86637200000001</v>
+      </c>
+      <c r="H38" t="s">
+        <v>70</v>
+      </c>
+      <c r="I38" s="1" t="str">
+        <f>CONCATENATE(H38," ",A38)</f>
+        <v>Sydney 34</v>
+      </c>
+      <c r="J38" t="s">
+        <v>78</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L38" t="s">
+        <v>79</v>
+      </c>
+      <c r="M38" t="s">
+        <v>80</v>
+      </c>
+      <c r="N38" t="s">
+        <v>81</v>
+      </c>
+      <c r="O38" t="s">
+        <v>75</v>
+      </c>
+      <c r="P38" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'Sydney 34',start_avail,end_avail,color_str='0,255,255,100',lower_lat=-35.955051,upper_lat=-31.955051,left_long=148.866372,right_long=152.866372)</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
+      <c r="A39" s="1">
+        <v>35</v>
+      </c>
+      <c r="B39">
+        <v>-31.91244</v>
+      </c>
+      <c r="C39">
+        <v>116.73866200000001</v>
+      </c>
+      <c r="D39" s="1">
+        <f>B39+$A$2</f>
+        <v>-33.912440000000004</v>
+      </c>
+      <c r="E39" s="1">
+        <f>B39+$B$2</f>
+        <v>-29.91244</v>
+      </c>
+      <c r="F39" s="1">
+        <f>C39+$C$2</f>
+        <v>114.73866200000001</v>
+      </c>
+      <c r="G39" s="1">
+        <f>C39+$D$2</f>
+        <v>118.73866200000001</v>
+      </c>
+      <c r="H39" t="s">
+        <v>71</v>
+      </c>
+      <c r="I39" s="1" t="str">
+        <f>CONCATENATE(H39," ",A39)</f>
+        <v>Perth 35</v>
+      </c>
+      <c r="J39" t="s">
+        <v>78</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L39" t="s">
+        <v>79</v>
+      </c>
+      <c r="M39" t="s">
+        <v>80</v>
+      </c>
+      <c r="N39" t="s">
+        <v>81</v>
+      </c>
+      <c r="O39" t="s">
+        <v>75</v>
+      </c>
+      <c r="P39" t="str">
+        <f t="shared" si="0"/>
+        <v>cztl.writeObsTextRect(all_fd,'Perth 35',start_avail,end_avail,color_str='0,255,255,100',lower_lat=-33.91244,upper_lat=-29.91244,left_long=114.738662,right_long=118.738662)</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="I46" s="1"/>
+    </row>
+    <row r="47" spans="1:16">
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="I47" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>